<commit_message>
study 3 set up, study 4 almost study 2 just added
</commit_message>
<xml_diff>
--- a/Study 3/Models_link/Sets/Regions.xlsx
+++ b/Study 3/Models_link/Sets/Regions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\IAM-COMPACT\Models_link\Sets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\IAM_COMPACT_1stMC\Study 3\Models_link\Sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8E55DB-C6C6-408A-8647-3F9F592C34D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C90C6-6524-4DFD-B83B-6EAD1E3DEB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GCAM" sheetId="1" r:id="rId1"/>
@@ -188,10 +188,10 @@
     <t>European Free Trade Association</t>
   </si>
   <si>
+    <t>RoW</t>
+  </si>
+  <si>
     <t>EU27</t>
-  </si>
-  <si>
-    <t>RoW</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>